<commit_message>
test loader and builder
</commit_message>
<xml_diff>
--- a/CarPark/src/test/resources/Automobiles.xlsx
+++ b/CarPark/src/test/resources/Automobiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\training\PolimorfismAutoIO\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\training\CarPark\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="car" sheetId="1" r:id="rId1"/>
-    <sheet name="#truck" sheetId="2" r:id="rId2"/>
-    <sheet name="trucks" sheetId="3" r:id="rId3"/>
+    <sheet name="trucks" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -123,12 +122,24 @@
   <si>
     <t>BPW</t>
   </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Camry</t>
+  </si>
+  <si>
+    <t>COUPE</t>
+  </si>
+  <si>
+    <t>B1997</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +163,6 @@
       <family val="3"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,12 +184,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -473,7 +476,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,6 +561,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3456778</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>230</v>
+      </c>
+      <c r="E4">
+        <v>34000.800000000003</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
     </row>
@@ -569,147 +595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>129908</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>330</v>
-      </c>
-      <c r="E2">
-        <v>40333.800000000003</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2">
-        <v>120</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>343890</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>320</v>
-      </c>
-      <c r="E3">
-        <v>65056.6</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1997</v>
-      </c>
-      <c r="H3">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>92</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="F9" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,10 +631,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -777,10 +666,10 @@
       <c r="E2">
         <v>43988.800000000003</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H2">
@@ -793,6 +682,41 @@
         <v>22</v>
       </c>
       <c r="K2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>343890</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>320</v>
+      </c>
+      <c r="E3">
+        <v>65056.6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>92</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>